<commit_message>
Conceptual figure and functional groups
Snip and sketch the conceptual figure from the Powerpoint. Edited the Excel file where I assign compounds to different parts of the IR spectra
</commit_message>
<xml_diff>
--- a/Metadata/Compounds classified by functional groups.xlsx
+++ b/Metadata/Compounds classified by functional groups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial-enzyme-activity-in-leaf-litter\Metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F80771-E87D-417F-A13C-BBBBE308D59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5FAA06-C87B-4B19-BF5B-62B4AF19E1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3DDBC223-3093-497B-913B-C132E43F0BE6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3DDBC223-3093-497B-913B-C132E43F0BE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,20 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>FTIR spectral range</t>
   </si>
   <si>
-    <t>Original name</t>
-  </si>
-  <si>
-    <t>New name</t>
-  </si>
-  <si>
-    <t>Functional group</t>
-  </si>
-  <si>
     <t>Compound</t>
   </si>
   <si>
@@ -61,12 +52,6 @@
     <t>carboEster1</t>
   </si>
   <si>
-    <t>carbohydrate esters</t>
-  </si>
-  <si>
-    <t>hemicellulose, pectins</t>
-  </si>
-  <si>
     <t>1015 - 1080</t>
   </si>
   <si>
@@ -76,9 +61,6 @@
     <t>glycosidicBond</t>
   </si>
   <si>
-    <t>glycosidic bonds</t>
-  </si>
-  <si>
     <t>1100 - 1160</t>
   </si>
   <si>
@@ -97,52 +79,88 @@
     <t>C_O_stretching</t>
   </si>
   <si>
-    <t>carbohydrate C-O stretches</t>
-  </si>
-  <si>
-    <t>all carbohydrates (complex carbohydrates + oligosaccharides + monosaccharides)</t>
-  </si>
-  <si>
     <t>1450 - 1475</t>
   </si>
   <si>
     <t>alkane</t>
   </si>
   <si>
-    <t>single bonds</t>
-  </si>
-  <si>
     <t>1545 - 1600</t>
   </si>
   <si>
     <t>amide1</t>
   </si>
   <si>
-    <t>amide</t>
-  </si>
-  <si>
-    <t>proteins</t>
-  </si>
-  <si>
     <t>1620 - 1645</t>
   </si>
   <si>
     <t>amide2</t>
   </si>
   <si>
-    <t>cellulose, simple sugars (oligosaccharides + monosaccharides)</t>
-  </si>
-  <si>
-    <t>complex carbohydrates (hemicellulose + pectins + cellulose)</t>
-  </si>
-  <si>
     <t>1700 - 1750</t>
   </si>
   <si>
     <t>lipid</t>
   </si>
   <si>
-    <t>Check for other compounds</t>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Madari et al 2006; Zhuang et al 2020</t>
+  </si>
+  <si>
+    <t>Madari et al 2006</t>
+  </si>
+  <si>
+    <t>Zhuang et al 2020</t>
+  </si>
+  <si>
+    <t>Lignin</t>
+  </si>
+  <si>
+    <t>Hemicellulose, Pectins</t>
+  </si>
+  <si>
+    <t>All carbohydrates</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Hemicellulose, Lignin</t>
+  </si>
+  <si>
+    <t>Cellulose, Hemicellulose, Lignin</t>
+  </si>
+  <si>
+    <t>Band assignment</t>
+  </si>
+  <si>
+    <t>C-O stretching of esters</t>
+  </si>
+  <si>
+    <t>C-O deformation of glycosidic bonds</t>
+  </si>
+  <si>
+    <t>Amide</t>
+  </si>
+  <si>
+    <t>C-H deformation in methyl and methylene</t>
+  </si>
+  <si>
+    <t>Name given by Ashish</t>
+  </si>
+  <si>
+    <t>Original name in data analysis</t>
+  </si>
+  <si>
+    <t>Band number</t>
+  </si>
+  <si>
+    <t>C=O stretching</t>
+  </si>
+  <si>
+    <t>C-O stretches</t>
   </si>
 </sst>
 </file>
@@ -212,10 +230,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -531,175 +551,228 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A10867-1465-4D7F-8A5B-DAA96555E92C}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>